<commit_message>
15:00 - 28/04 - DB erstellt und Upserts festgstellt
</commit_message>
<xml_diff>
--- a/data/Upserts/Upserts.xlsx
+++ b/data/Upserts/Upserts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIT5LO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\schrauber_Verwaltung\data\Upserts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A6EC12F-38BE-4586-988F-DA42C90DDF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F92C7-821D-4A72-8029-86D72CDF3DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E7BED24-DB63-4ECE-B973-C7BA53D25068}"/>
   </bookViews>
@@ -1179,7 +1179,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1216,7 +1216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42" customHeight="1">
+    <row r="2" spans="1:7" ht="49.5" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42" customHeight="1">
+    <row r="3" spans="1:7" ht="61.5" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42" customHeight="1">
+    <row r="4" spans="1:7" ht="49.5" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42" customHeight="1">
+    <row r="5" spans="1:7" ht="49.5" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="42" customHeight="1">
+    <row r="6" spans="1:7" ht="49.5" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42" customHeight="1">
+    <row r="7" spans="1:7" ht="49.5" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42" customHeight="1">
+    <row r="8" spans="1:7" ht="49.5" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="42" customHeight="1">
+    <row r="9" spans="1:7" ht="49.5" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="42" customHeight="1">
+    <row r="10" spans="1:7" ht="49.5" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>

</xml_diff>